<commit_message>
Further cleaning of subsampling code and update of ground truth detection points for validation set (33 entries so far)
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts.xlsx
+++ b/GHT/ground_truth_detection_pts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 1\ESC499 - Thesis\Undergraduate_Thesis_Scripts\GHT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\ESC499 - Thesis\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBE035E-401E-4168-9A9C-DB9AD22C40BE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1EBB8B-6D64-479E-98AF-F848B0E9C375}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>x is left to right, y is up to down, z is into the page</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>x</t>
   </si>
@@ -51,7 +48,34 @@
     <t>Accession Num</t>
   </si>
   <si>
-    <t>Didn't have any record</t>
+    <t>x is top to bottom, y is left to right, z is out of the page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>This one is big in scale</t>
+  </si>
+  <si>
+    <t>This one is small in scale</t>
+  </si>
+  <si>
+    <t>Incredibly Small</t>
+  </si>
+  <si>
+    <t>Rotated around 10 degrees</t>
+  </si>
+  <si>
+    <t>Very big</t>
+  </si>
+  <si>
+    <t>Big in scale</t>
+  </si>
+  <si>
+    <t>Rotated around 10 degrees ccw</t>
+  </si>
+  <si>
+    <t>Terrible</t>
   </si>
 </sst>
 </file>
@@ -424,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -437,469 +461,555 @@
     <col min="5" max="5" width="54.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>4491140</v>
+        <v>4687879</v>
       </c>
       <c r="B3" s="2">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>4787879</v>
+        <v>5056218</v>
       </c>
       <c r="B4" s="2">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>5056218</v>
+        <v>5199556</v>
       </c>
       <c r="B5" s="2">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5235783</v>
+      </c>
+      <c r="B6" s="2">
+        <v>35</v>
+      </c>
+      <c r="C6" s="2">
+        <v>57</v>
+      </c>
+      <c r="D6" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>5199556</v>
-      </c>
-      <c r="B6" s="2">
-        <v>45</v>
-      </c>
-      <c r="C6" s="2">
-        <v>54</v>
-      </c>
-      <c r="D6" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>5235783</v>
+        <v>5372580</v>
       </c>
       <c r="B7" s="2">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>5372580</v>
+        <v>5433681</v>
       </c>
       <c r="B8" s="2">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2">
+        <v>65</v>
+      </c>
+      <c r="D8" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>5506328</v>
+      </c>
+      <c r="B9" s="2">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2">
+        <v>46</v>
+      </c>
+      <c r="D9" s="2">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>5523521</v>
+      </c>
+      <c r="B10" s="2">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43</v>
+      </c>
+      <c r="D10" s="2">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>5680178</v>
+      </c>
+      <c r="B11" s="2">
         <v>31</v>
       </c>
-      <c r="C8" s="2">
-        <v>50</v>
-      </c>
-      <c r="D8" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>5433681</v>
-      </c>
-      <c r="B9" s="2">
-        <v>41</v>
-      </c>
-      <c r="C9" s="2">
-        <v>65</v>
-      </c>
-      <c r="D9" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>5506328</v>
-      </c>
-      <c r="B10" s="2">
-        <v>26</v>
-      </c>
-      <c r="C10" s="2">
-        <v>45</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C11" s="2">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>5739421</v>
+      </c>
+      <c r="B12" s="2">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2">
+        <v>60</v>
+      </c>
+      <c r="D12" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>5523521</v>
-      </c>
-      <c r="B11" s="2">
-        <v>26</v>
-      </c>
-      <c r="C11" s="2">
-        <v>45</v>
-      </c>
-      <c r="D11" s="2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>5826444</v>
+      </c>
+      <c r="B13" s="2">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2">
+        <v>57</v>
+      </c>
+      <c r="D13" s="2">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>5835023</v>
+      </c>
+      <c r="B14" s="2">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2">
+        <v>63</v>
+      </c>
+      <c r="D14" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
-        <v>5680178</v>
-      </c>
-      <c r="B12" s="2">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2">
-        <v>55</v>
-      </c>
-      <c r="D12" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
-        <v>5739421</v>
-      </c>
-      <c r="B13" s="2">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2">
-        <v>58</v>
-      </c>
-      <c r="D13" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
-        <v>5826444</v>
-      </c>
-      <c r="B14" s="2">
-        <v>41</v>
-      </c>
-      <c r="C14" s="2">
-        <v>54</v>
-      </c>
-      <c r="D14" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>5835023</v>
+        <v>6022046</v>
       </c>
       <c r="B15" s="2">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D15" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>6022046</v>
+        <v>6029287</v>
       </c>
       <c r="B16" s="2">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D16" s="2">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>6029287</v>
-      </c>
-      <c r="B17" s="2">
-        <v>38</v>
-      </c>
-      <c r="C17" s="2">
-        <v>51</v>
-      </c>
-      <c r="D17" s="2">
-        <v>15</v>
+        <v>6055185</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>6055185</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" t="s">
-        <v>6</v>
+        <v>6067977</v>
+      </c>
+      <c r="B18" s="2">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2">
+        <v>58</v>
+      </c>
+      <c r="D18" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>6067977</v>
+        <v>6095054</v>
       </c>
       <c r="B19" s="2">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>6095054</v>
-      </c>
-      <c r="B20" s="2">
-        <v>32</v>
-      </c>
-      <c r="C20" s="2">
-        <v>41</v>
-      </c>
-      <c r="D20" s="2">
-        <v>23</v>
-      </c>
+        <v>6165341</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>6165341</v>
+        <v>6173842</v>
       </c>
       <c r="B21" s="2">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C21" s="2">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>6173842</v>
+        <v>6201211</v>
       </c>
       <c r="B22" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>6201211</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+        <v>6218246</v>
+      </c>
+      <c r="B23" s="2">
+        <v>29</v>
+      </c>
+      <c r="C23" s="2">
+        <v>61</v>
+      </c>
+      <c r="D23" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>6218246</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+        <v>6268647</v>
+      </c>
+      <c r="B24" s="2">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2">
+        <v>47</v>
+      </c>
+      <c r="D24" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
-        <v>6254655</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+        <v>6490491</v>
+      </c>
+      <c r="B25" s="2">
+        <v>30</v>
+      </c>
+      <c r="C25" s="2">
+        <v>54</v>
+      </c>
+      <c r="D25" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
-        <v>6268647</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+        <v>6729799</v>
+      </c>
+      <c r="B26" s="2">
+        <v>32</v>
+      </c>
+      <c r="C26" s="2">
+        <v>37</v>
+      </c>
+      <c r="D26" s="2">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
-        <v>6292201</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+        <v>6828936</v>
+      </c>
+      <c r="B27" s="2">
+        <v>27</v>
+      </c>
+      <c r="C27" s="2">
+        <v>47</v>
+      </c>
+      <c r="D27" s="2">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
-        <v>6490491</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+        <v>6868398</v>
+      </c>
+      <c r="B28" s="2">
+        <v>32</v>
+      </c>
+      <c r="C28" s="2">
+        <v>53</v>
+      </c>
+      <c r="D28" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
-        <v>6729799</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+        <v>6881614</v>
+      </c>
+      <c r="B29" s="2">
+        <v>29</v>
+      </c>
+      <c r="C29" s="2">
+        <v>55</v>
+      </c>
+      <c r="D29" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
-        <v>6828936</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+        <v>6993961</v>
+      </c>
+      <c r="B30" s="2">
+        <v>31</v>
+      </c>
+      <c r="C30" s="2">
+        <v>63</v>
+      </c>
+      <c r="D30" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
-        <v>6868398</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+        <v>7081341</v>
+      </c>
+      <c r="B31" s="2">
+        <v>29</v>
+      </c>
+      <c r="C31" s="2">
+        <v>51</v>
+      </c>
+      <c r="D31" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
-        <v>6881614</v>
+        <v>7202530</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
+      <c r="E32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
-        <v>6973272</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+        <v>7222303</v>
+      </c>
+      <c r="B33" s="2">
+        <v>32</v>
+      </c>
+      <c r="C33" s="2">
+        <v>51</v>
+      </c>
+      <c r="D33" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
-        <v>6993961</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+        <v>7257259</v>
+      </c>
+      <c r="B34" s="2">
+        <v>29</v>
+      </c>
+      <c r="C34" s="2">
+        <v>57</v>
+      </c>
+      <c r="D34" s="2">
+        <v>24</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
-        <v>7081341</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+        <v>7299268</v>
+      </c>
+      <c r="B35" s="2">
+        <v>26</v>
+      </c>
+      <c r="C35" s="2">
+        <v>59</v>
+      </c>
+      <c r="D35" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
-        <v>7205230</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+        <v>7316415</v>
+      </c>
+      <c r="B36" s="2">
+        <v>32</v>
+      </c>
+      <c r="C36" s="2">
+        <v>63</v>
+      </c>
+      <c r="D36" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
-        <v>7222303</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+        <v>7337296</v>
+      </c>
+      <c r="B37" s="2">
+        <v>32</v>
+      </c>
+      <c r="C37" s="2">
+        <v>51</v>
+      </c>
+      <c r="D37" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
-        <v>7257259</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+        <v>7396455</v>
+      </c>
+      <c r="B38" s="2">
+        <v>48</v>
+      </c>
+      <c r="C38" s="2">
+        <v>54</v>
+      </c>
+      <c r="D38" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
-        <v>7299268</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="2">
-        <v>7316415</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="2">
-        <v>7337296</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="2">
-        <v>7396455</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E13">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E12">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>

<commit_message>
40 ground truth points
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts.xlsx
+++ b/GHT/ground_truth_detection_pts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\ESC499 - Thesis\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1EBB8B-6D64-479E-98AF-F848B0E9C375}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9458D63D-EE36-4B7B-A52A-B5F401FB1AA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>x</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Terrible</t>
+  </si>
+  <si>
+    <t>A bit light of a picture</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -919,7 +922,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>7222303</v>
       </c>
@@ -933,7 +936,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>7257259</v>
       </c>
@@ -947,7 +950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>7299268</v>
       </c>
@@ -961,7 +964,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>7316415</v>
       </c>
@@ -975,7 +978,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>7337296</v>
       </c>
@@ -989,7 +992,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>7396455</v>
       </c>
@@ -1003,8 +1006,104 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
+        <v>7444276</v>
+      </c>
+      <c r="B39" s="2">
+        <v>26</v>
+      </c>
+      <c r="C39" s="2">
+        <v>50</v>
+      </c>
+      <c r="D39" s="2">
+        <v>19</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>7466141</v>
+      </c>
+      <c r="B40" s="2">
+        <v>29</v>
+      </c>
+      <c r="C40" s="2">
+        <v>62</v>
+      </c>
+      <c r="D40" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>7489680</v>
+      </c>
+      <c r="B41" s="2">
+        <v>33</v>
+      </c>
+      <c r="C41" s="2">
+        <v>53</v>
+      </c>
+      <c r="D41" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>7496249</v>
+      </c>
+      <c r="B42" s="2">
+        <v>23</v>
+      </c>
+      <c r="C42" s="2">
+        <v>51</v>
+      </c>
+      <c r="D42" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>7499820</v>
+      </c>
+      <c r="B43" s="2">
+        <v>33</v>
+      </c>
+      <c r="C43" s="2">
+        <v>49</v>
+      </c>
+      <c r="D43" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>7629097</v>
+      </c>
+      <c r="B44" s="2">
+        <v>33</v>
+      </c>
+      <c r="C44" s="2">
+        <v>42</v>
+      </c>
+      <c r="D44" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>7796800</v>
+      </c>
+      <c r="B45" s="2">
+        <v>29</v>
+      </c>
+      <c r="C45" s="2">
+        <v>52</v>
+      </c>
+      <c r="D45" s="2">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating to more accurate ground truth
</commit_message>
<xml_diff>
--- a/GHT/ground_truth_detection_pts.xlsx
+++ b/GHT/ground_truth_detection_pts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoons\Documents\4th Year Semester 2\ESC499 - Thesis\Undergraduate_Thesis_Scripts\GHT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9458D63D-EE36-4B7B-A52A-B5F401FB1AA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DFF4C1-BFB2-4E7F-8671-C87E57578450}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12100" xr2:uid="{E54F2B35-E95B-4A69-BE1D-76005A0015F2}"/>
   </bookViews>
@@ -451,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5C2FB5-FE99-445B-85B0-EF4DB711D45B}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,69 +492,70 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>4687879</v>
+        <v>4491140</v>
       </c>
       <c r="B3" s="2">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>5056218</v>
+        <v>4687879</v>
       </c>
       <c r="B4" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>5199556</v>
+        <v>5056218</v>
       </c>
       <c r="B5" s="2">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>5235783</v>
+        <v>5199556</v>
       </c>
       <c r="B6" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>5372580</v>
+        <v>5235783</v>
       </c>
       <c r="B7" s="2">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D7" s="2">
         <v>19</v>
@@ -562,322 +563,322 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>5433681</v>
+        <v>5372580</v>
       </c>
       <c r="B8" s="2">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>5506328</v>
+        <v>5433681</v>
       </c>
       <c r="B9" s="2">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>5523521</v>
+        <v>5506328</v>
       </c>
       <c r="B10" s="2">
         <v>28</v>
       </c>
       <c r="C10" s="2">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>5680178</v>
+        <v>5523521</v>
       </c>
       <c r="B11" s="2">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>5739421</v>
+        <v>5680178</v>
       </c>
       <c r="B12" s="2">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>5826444</v>
+        <v>5739421</v>
       </c>
       <c r="B13" s="2">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D13" s="2">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>5835023</v>
+        <v>5826444</v>
       </c>
       <c r="B14" s="2">
         <v>34</v>
       </c>
       <c r="C14" s="2">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>6022046</v>
+        <v>5835023</v>
       </c>
       <c r="B15" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D15" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>6029287</v>
+        <v>6022046</v>
       </c>
       <c r="B16" s="2">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C16" s="2">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D16" s="2">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>6055185</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" t="s">
-        <v>9</v>
+        <v>6029287</v>
+      </c>
+      <c r="B17" s="2">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2">
+        <v>53</v>
+      </c>
+      <c r="D17" s="2">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>6067977</v>
-      </c>
-      <c r="B18" s="2">
-        <v>35</v>
-      </c>
-      <c r="C18" s="2">
-        <v>58</v>
-      </c>
-      <c r="D18" s="2">
-        <v>18</v>
+        <v>6055185</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>6095054</v>
+        <v>6067977</v>
       </c>
       <c r="B19" s="2">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="D19" s="2">
-        <v>25</v>
-      </c>
-      <c r="E19" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>6165341</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+        <v>6095054</v>
+      </c>
+      <c r="B20" s="2">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2">
+        <v>43</v>
+      </c>
+      <c r="D20" s="2">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>6173842</v>
-      </c>
-      <c r="B21" s="2">
-        <v>29</v>
-      </c>
-      <c r="C21" s="2">
-        <v>56</v>
-      </c>
-      <c r="D21" s="2">
-        <v>18</v>
-      </c>
+        <v>6165341</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>6201211</v>
+        <v>6173842</v>
       </c>
       <c r="B22" s="2">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C22" s="2">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2">
-        <v>17</v>
-      </c>
-      <c r="E22" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>6218246</v>
+        <v>6201211</v>
       </c>
       <c r="B23" s="2">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D23" s="2">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>6268647</v>
+        <v>6218246</v>
       </c>
       <c r="B24" s="2">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C24" s="2">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D24" s="2">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
-        <v>6490491</v>
+        <v>6268647</v>
       </c>
       <c r="B25" s="2">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C25" s="2">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D25" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
-        <v>6729799</v>
+        <v>6490491</v>
       </c>
       <c r="B26" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26" s="2">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="D26" s="2">
         <v>19</v>
       </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
-        <v>6828936</v>
+        <v>6729799</v>
       </c>
       <c r="B27" s="2">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D27" s="2">
         <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
-        <v>6868398</v>
+        <v>6828936</v>
       </c>
       <c r="B28" s="2">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C28" s="2">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D28" s="2">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
-        <v>6881614</v>
+        <v>6868398</v>
       </c>
       <c r="B29" s="2">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C29" s="2">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29" s="2">
         <v>20</v>
@@ -885,94 +886,94 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
-        <v>6993961</v>
+        <v>6881614</v>
       </c>
       <c r="B30" s="2">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" s="2">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D30" s="2">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
-        <v>7081341</v>
+        <v>6993961</v>
       </c>
       <c r="B31" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C31" s="2">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D31" s="2">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
-        <v>7202530</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" t="s">
-        <v>14</v>
+        <v>7081341</v>
+      </c>
+      <c r="B32" s="2">
+        <v>29</v>
+      </c>
+      <c r="C32" s="2">
+        <v>51</v>
+      </c>
+      <c r="D32" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
-        <v>7222303</v>
-      </c>
-      <c r="B33" s="2">
-        <v>32</v>
-      </c>
-      <c r="C33" s="2">
-        <v>51</v>
-      </c>
-      <c r="D33" s="2">
-        <v>17</v>
+        <v>7202530</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
-        <v>7257259</v>
+        <v>7222303</v>
       </c>
       <c r="B34" s="2">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C34" s="2">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D34" s="2">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
-        <v>7299268</v>
+        <v>7257259</v>
       </c>
       <c r="B35" s="2">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C35" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D35" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
-        <v>7316415</v>
+        <v>7299268</v>
       </c>
       <c r="B36" s="2">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C36" s="2">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D36" s="2">
         <v>23</v>
@@ -980,13 +981,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
-        <v>7337296</v>
+        <v>7316415</v>
       </c>
       <c r="B37" s="2">
         <v>32</v>
       </c>
       <c r="C37" s="2">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D37" s="2">
         <v>23</v>
@@ -994,86 +995,86 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
-        <v>7396455</v>
+        <v>7337296</v>
       </c>
       <c r="B38" s="2">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C38" s="2">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D38" s="2">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
-        <v>7444276</v>
+        <v>7396455</v>
       </c>
       <c r="B39" s="2">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C39" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D39" s="2">
-        <v>19</v>
-      </c>
-      <c r="E39" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
-        <v>7466141</v>
+        <v>7444276</v>
       </c>
       <c r="B40" s="2">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C40" s="2">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D40" s="2">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="E40" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
-        <v>7489680</v>
+        <v>7466141</v>
       </c>
       <c r="B41" s="2">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C41" s="2">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D41" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
-        <v>7496249</v>
+        <v>7489680</v>
       </c>
       <c r="B42" s="2">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C42" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D42" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
-        <v>7499820</v>
+        <v>7496249</v>
       </c>
       <c r="B43" s="2">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C43" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D43" s="2">
         <v>21</v>
@@ -1081,35 +1082,49 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
-        <v>7629097</v>
+        <v>7499820</v>
       </c>
       <c r="B44" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C44" s="2">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D44" s="2">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
+        <v>7629097</v>
+      </c>
+      <c r="B45" s="2">
+        <v>33</v>
+      </c>
+      <c r="C45" s="2">
+        <v>42</v>
+      </c>
+      <c r="D45" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
         <v>7796800</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B46" s="2">
         <v>29</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C46" s="2">
         <v>52</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D46" s="2">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E12">
-    <sortCondition ref="A3"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E13">
+    <sortCondition ref="A4"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>